<commit_message>
Getting ready to reboot to attempt to fix Excel scope reading document error.
</commit_message>
<xml_diff>
--- a/InputReceipt.xlsx
+++ b/InputReceipt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\UiPath\Jupyter Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8836E896-9FCA-4135-9030-DA5C1C707544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CCA9D0-9B4A-4FF6-9E23-EE6E8574B47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="75" windowWidth="13485" windowHeight="10410" activeTab="1" xr2:uid="{2ED60EC7-2034-47C9-A7E7-28EA61D7A613}"/>
+    <workbookView xWindow="1035" yWindow="1530" windowWidth="13485" windowHeight="13575" xr2:uid="{2ED60EC7-2034-47C9-A7E7-28EA61D7A613}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Matches</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>ghi</t>
+  </si>
+  <si>
+    <t>Break Out</t>
   </si>
 </sst>
 </file>
@@ -427,9 +430,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A044E7F7-DDA1-4D06-829C-5403DEA70DC0}">
-  <dimension ref="A4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -438,6 +441,11 @@
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
     </row>
@@ -450,7 +458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CC961F-04C5-436E-9E75-4766A4A8E356}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>